<commit_message>
Final project primera versión 21/10
</commit_message>
<xml_diff>
--- a/Encuesta sobre hábitos de deporte - Survey on sports habits (respuestas).xlsx
+++ b/Encuesta sobre hábitos de deporte - Survey on sports habits (respuestas).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://urjc-my.sharepoint.com/personal/v_anguix_2019_alumnos_urjc_es/Documents/Escritorio/MASTER/Statistics for data analysis/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://urjc-my.sharepoint.com/personal/v_anguix_2019_alumnos_urjc_es/Documents/Escritorio/MASTER/Statistics for data analysis/Project/Statistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_CD88C816998DA4A7E5C66D37C92528E350C36241" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51AD6093-7B79-4C02-BBE3-11899F503B23}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_CD88C816998DA4A7E5C66D37C92528E350C36241" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A742F6E4-62C3-4330-B8F6-7F3E016DA94F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -616,10 +616,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -826,8 +822,8 @@
   <dimension ref="A1:I174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D159" sqref="D159"/>
+      <pane ySplit="1" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:A175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3330,15 +3326,40 @@
       </c>
     </row>
     <row r="87" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="2"/>
-      <c r="B87" s="3"/>
+      <c r="A87" s="2">
+        <v>45196.748838622691</v>
+      </c>
+      <c r="B87" s="3">
+        <v>37012</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E87" s="1">
+        <v>2</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G87" s="1">
+        <v>150</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="88" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>45196.748838622691</v>
+        <v>45196.749004120371</v>
       </c>
       <c r="B88" s="3">
-        <v>37012</v>
+        <v>37170</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>14</v>
@@ -3347,161 +3368,161 @@
         <v>10</v>
       </c>
       <c r="E88" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>106</v>
+        <v>11</v>
       </c>
       <c r="G88" s="1">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>45196.749004120371</v>
+        <v>45196.752412766204</v>
       </c>
       <c r="B89" s="3">
-        <v>37170</v>
+        <v>24465</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="E89" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="G89" s="1">
-        <v>300</v>
+        <v>6</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>45196.752412766204</v>
+        <v>45196.758245844903</v>
       </c>
       <c r="B90" s="3">
-        <v>24465</v>
+        <v>37463</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E90" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="G90" s="1">
-        <v>6</v>
+        <v>400</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>45196.758245844903</v>
+        <v>45196.758730960646</v>
       </c>
       <c r="B91" s="3">
-        <v>37463</v>
+        <v>34459</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E91" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="G91" s="1">
-        <v>400</v>
+        <v>7</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>45196.758730960646</v>
+        <v>45196.761693518521</v>
       </c>
       <c r="B92" s="3">
-        <v>34459</v>
+        <v>24953</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E92" s="1">
         <v>2</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="G92" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>108</v>
+        <v>21</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>45196.761693518521</v>
+        <v>45196.762469270834</v>
       </c>
       <c r="B93" s="3">
-        <v>24953</v>
+        <v>24473</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E93" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>109</v>
+        <v>66</v>
       </c>
       <c r="G93" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I93" s="1" t="s">
         <v>13</v>
@@ -3509,71 +3530,71 @@
     </row>
     <row r="94" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>45196.762469270834</v>
+        <v>45196.762691909724</v>
       </c>
       <c r="B94" s="3">
-        <v>24473</v>
+        <v>22744</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E94" s="1">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="G94" s="1">
-        <v>180</v>
+        <v>1200</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>17</v>
+        <v>94</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>45196.762691909724</v>
+        <v>45196.766618981477</v>
       </c>
       <c r="B95" s="3">
-        <v>22744</v>
+        <v>25939</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>47</v>
+        <v>10</v>
+      </c>
+      <c r="E95" s="1">
+        <v>1</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="G95" s="1">
-        <v>1200</v>
+        <v>120</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>94</v>
+        <v>17</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>45196.766618981477</v>
+        <v>45196.771378159727</v>
       </c>
       <c r="B96" s="3">
-        <v>25939</v>
+        <v>30937</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>10</v>
@@ -3582,24 +3603,24 @@
         <v>1</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="G96" s="1">
-        <v>120</v>
+        <v>4</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>45196.771378159727</v>
+        <v>45196.781749849542</v>
       </c>
       <c r="B97" s="3">
-        <v>30937</v>
+        <v>22935</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>9</v>
@@ -3608,30 +3629,30 @@
         <v>10</v>
       </c>
       <c r="E97" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>45</v>
+        <v>111</v>
       </c>
       <c r="G97" s="1">
-        <v>4</v>
+        <v>250</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>45196.781749849542</v>
+        <v>45196.790350671297</v>
       </c>
       <c r="B98" s="3">
-        <v>22935</v>
+        <v>28301</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>10</v>
@@ -3640,42 +3661,42 @@
         <v>2</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>111</v>
+        <v>45</v>
       </c>
       <c r="G98" s="1">
-        <v>250</v>
+        <v>180</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>25</v>
+        <v>112</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>45196.790350671297</v>
+        <v>45196.792820127317</v>
       </c>
       <c r="B99" s="3">
-        <v>28301</v>
+        <v>23767</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="E99" s="1">
         <v>2</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G99" s="1">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I99" s="1" t="s">
         <v>13</v>
@@ -3683,10 +3704,10 @@
     </row>
     <row r="100" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>45196.792820127317</v>
+        <v>45196.795588668982</v>
       </c>
       <c r="B100" s="3">
-        <v>23767</v>
+        <v>28472</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>9</v>
@@ -3698,24 +3719,24 @@
         <v>2</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>51</v>
+        <v>114</v>
       </c>
       <c r="G100" s="1">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>45196.795588668982</v>
+        <v>45196.798030347221</v>
       </c>
       <c r="B101" s="3">
-        <v>28472</v>
+        <v>32673</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>9</v>
@@ -3723,17 +3744,17 @@
       <c r="D101" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E101" s="1">
-        <v>2</v>
+      <c r="E101" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G101" s="1">
-        <v>600</v>
+        <v>115</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="I101" s="1" t="s">
         <v>22</v>
@@ -3741,13 +3762,13 @@
     </row>
     <row r="102" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>45196.798030347221</v>
+        <v>45196.799252187498</v>
       </c>
       <c r="B102" s="3">
-        <v>32673</v>
+        <v>31027</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>32</v>
@@ -3756,24 +3777,24 @@
         <v>47</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G102" s="1" t="s">
-        <v>116</v>
+        <v>18</v>
+      </c>
+      <c r="G102" s="1">
+        <v>10</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>45196.799252187498</v>
+        <v>45196.805723425925</v>
       </c>
       <c r="B103" s="3">
-        <v>31027</v>
+        <v>27759</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>14</v>
@@ -3788,50 +3809,50 @@
         <v>18</v>
       </c>
       <c r="G103" s="1">
-        <v>10</v>
+        <v>360</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
-        <v>45196.805723425925</v>
+        <v>45196.809309907403</v>
       </c>
       <c r="B104" s="3">
-        <v>27759</v>
+        <v>29339</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>18</v>
+        <v>119</v>
       </c>
       <c r="G104" s="1">
-        <v>360</v>
+        <v>10</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
-        <v>45196.809309907403</v>
+        <v>45196.811861539347</v>
       </c>
       <c r="B105" s="3">
-        <v>29339</v>
+        <v>27894</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>14</v>
@@ -3839,17 +3860,17 @@
       <c r="D105" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E105" s="1" t="s">
-        <v>47</v>
+      <c r="E105" s="1">
+        <v>1</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G105" s="1">
-        <v>10</v>
+        <v>45</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>120</v>
+        <v>54</v>
       </c>
       <c r="I105" s="1" t="s">
         <v>13</v>
@@ -3857,10 +3878,10 @@
     </row>
     <row r="106" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
-        <v>45196.811861539347</v>
+        <v>45196.821618240741</v>
       </c>
       <c r="B106" s="3">
-        <v>27894</v>
+        <v>28277</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>14</v>
@@ -3869,16 +3890,16 @@
         <v>10</v>
       </c>
       <c r="E106" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>121</v>
+        <v>82</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>54</v>
+        <v>123</v>
       </c>
       <c r="I106" s="1" t="s">
         <v>13</v>
@@ -3886,28 +3907,28 @@
     </row>
     <row r="107" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
-        <v>45196.821618240741</v>
+        <v>45196.825294097223</v>
       </c>
       <c r="B107" s="3">
-        <v>28277</v>
+        <v>22120</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E107" s="1">
-        <v>2</v>
+        <v>32</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G107" s="1" t="s">
-        <v>82</v>
+        <v>124</v>
+      </c>
+      <c r="G107" s="1">
+        <v>400</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="I107" s="1" t="s">
         <v>13</v>
@@ -3915,155 +3936,155 @@
     </row>
     <row r="108" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
-        <v>45196.825294097223</v>
+        <v>45196.835279583334</v>
       </c>
       <c r="B108" s="3">
-        <v>22120</v>
+        <v>27869</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>47</v>
+        <v>10</v>
+      </c>
+      <c r="E108" s="1">
+        <v>2</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G108" s="1">
-        <v>400</v>
+        <v>51</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>101</v>
+        <v>39</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
-        <v>45196.835279583334</v>
+        <v>45196.836853668981</v>
       </c>
       <c r="B109" s="3">
-        <v>27869</v>
+        <v>27973</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E109" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G109" s="1" t="s">
-        <v>125</v>
+        <v>21</v>
+      </c>
+      <c r="G109" s="1">
+        <v>0</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
-        <v>45196.836853668981</v>
+        <v>45196.855648206023</v>
       </c>
       <c r="B110" s="3">
-        <v>27973</v>
+        <v>25738</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E110" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>21</v>
+        <v>126</v>
       </c>
       <c r="G110" s="1">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>21</v>
+        <v>120</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
-        <v>45196.855648206023</v>
+        <v>45196.856671898146</v>
       </c>
       <c r="B111" s="3">
-        <v>25738</v>
+        <v>25328</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E111" s="1">
         <v>2</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>126</v>
+        <v>11</v>
       </c>
       <c r="G111" s="1">
-        <v>360</v>
+        <v>180</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>120</v>
+        <v>54</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="112" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
-        <v>45196.856671898146</v>
+        <v>45196.859884618054</v>
       </c>
       <c r="B112" s="3">
-        <v>25328</v>
+        <v>26928</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="E112" s="1">
         <v>2</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G112" s="1">
-        <v>180</v>
+        <v>8</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
-        <v>45196.859884618054</v>
+        <v>45196.867669942134</v>
       </c>
       <c r="B113" s="3">
-        <v>26928</v>
+        <v>26640</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>9</v>
@@ -4071,31 +4092,31 @@
       <c r="D113" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E113" s="1">
-        <v>2</v>
+      <c r="E113" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>16</v>
+        <v>127</v>
       </c>
       <c r="G113" s="1">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="H113" s="1" t="s">
         <v>44</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
-        <v>45196.867669942134</v>
+        <v>45196.872701250002</v>
       </c>
       <c r="B114" s="3">
-        <v>26640</v>
+        <v>31891</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>32</v>
@@ -4104,56 +4125,56 @@
         <v>47</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G114" s="1">
-        <v>120</v>
+        <v>128</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
-        <v>45196.872701250002</v>
+        <v>45196.873166655088</v>
       </c>
       <c r="B115" s="3">
-        <v>31891</v>
+        <v>29254</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>47</v>
+        <v>10</v>
+      </c>
+      <c r="E115" s="1">
+        <v>2</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
+      </c>
+      <c r="G115" s="1">
+        <v>120</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
-        <v>45196.873166655088</v>
+        <v>45196.879770266205</v>
       </c>
       <c r="B116" s="3">
-        <v>29254</v>
+        <v>30670</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>10</v>
@@ -4162,30 +4183,30 @@
         <v>2</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>130</v>
+        <v>51</v>
       </c>
       <c r="G116" s="1">
-        <v>120</v>
+        <v>260</v>
       </c>
       <c r="H116" s="1" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
-        <v>45196.879770266205</v>
+        <v>45196.885760520832</v>
       </c>
       <c r="B117" s="3">
-        <v>30670</v>
+        <v>22976</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="E117" s="1">
         <v>2</v>
@@ -4194,50 +4215,50 @@
         <v>51</v>
       </c>
       <c r="G117" s="1">
-        <v>260</v>
+        <v>7</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
-        <v>45196.885760520832</v>
+        <v>45196.887005185185</v>
       </c>
       <c r="B118" s="3">
-        <v>22976</v>
+        <v>28490</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E118" s="1">
         <v>2</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G118" s="1">
-        <v>7</v>
+        <v>126</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
-        <v>45196.887005185185</v>
+        <v>45196.902772326386</v>
       </c>
       <c r="B119" s="3">
-        <v>28490</v>
+        <v>26567</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>14</v>
@@ -4246,59 +4267,59 @@
         <v>10</v>
       </c>
       <c r="E119" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>132</v>
+        <v>45</v>
+      </c>
+      <c r="G119" s="1">
+        <v>200</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
-        <v>45196.902772326386</v>
+        <v>45196.910721562497</v>
       </c>
       <c r="B120" s="3">
-        <v>26567</v>
+        <v>25575</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E120" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="G120" s="1">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>133</v>
+        <v>12</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
-        <v>45196.910721562497</v>
+        <v>45196.91214083333</v>
       </c>
       <c r="B121" s="3">
-        <v>25575</v>
+        <v>24700</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>10</v>
@@ -4310,21 +4331,21 @@
         <v>16</v>
       </c>
       <c r="G121" s="1">
-        <v>180</v>
+        <v>7</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="122" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
-        <v>45196.91214083333</v>
+        <v>45196.944293472217</v>
       </c>
       <c r="B122" s="3">
-        <v>24700</v>
+        <v>28778</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>14</v>
@@ -4339,39 +4360,39 @@
         <v>16</v>
       </c>
       <c r="G122" s="1">
-        <v>7</v>
+        <v>300</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
-        <v>45196.944293472217</v>
+        <v>45196.945778923611</v>
       </c>
       <c r="B123" s="3">
-        <v>28778</v>
+        <v>45020</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="E123" s="1">
         <v>2</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G123" s="1">
-        <v>300</v>
+        <v>81</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="I123" s="1" t="s">
         <v>13</v>
@@ -4379,68 +4400,68 @@
     </row>
     <row r="124" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
-        <v>45196.945778923611</v>
+        <v>45196.947641331019</v>
       </c>
       <c r="B124" s="3">
-        <v>45020</v>
+        <v>23932</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E124" s="1">
-        <v>2</v>
+      <c r="E124" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G124" s="1" t="s">
-        <v>132</v>
+        <v>51</v>
+      </c>
+      <c r="G124" s="1">
+        <v>600</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="125" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
-        <v>45196.947641331019</v>
+        <v>45196.951716898147</v>
       </c>
       <c r="B125" s="3">
-        <v>23932</v>
+        <v>28635</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E125" s="1" t="s">
-        <v>47</v>
+      <c r="E125" s="1">
+        <v>2</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G125" s="1">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>136</v>
+        <v>94</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
-        <v>45196.951716898147</v>
+        <v>45196.959275173613</v>
       </c>
       <c r="B126" s="3">
-        <v>28635</v>
+        <v>27370</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>14</v>
@@ -4448,75 +4469,75 @@
       <c r="D126" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E126" s="1">
-        <v>2</v>
+      <c r="E126" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>45</v>
+        <v>137</v>
       </c>
       <c r="G126" s="1">
-        <v>1200</v>
+        <v>14</v>
       </c>
       <c r="H126" s="1" t="s">
-        <v>94</v>
+        <v>138</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
-        <v>45196.959275173613</v>
+        <v>45196.967048877312</v>
       </c>
       <c r="B127" s="3">
-        <v>27370</v>
+        <v>30708</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
+      </c>
+      <c r="E127" s="1">
+        <v>1</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G127" s="1">
-        <v>14</v>
+        <v>180</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>138</v>
+        <v>54</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
-        <v>45196.967048877312</v>
+        <v>45196.970125578708</v>
       </c>
       <c r="B128" s="3">
-        <v>30708</v>
+        <v>27538</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E128" s="1">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G128" s="1">
-        <v>180</v>
+        <v>110</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="I128" s="1" t="s">
         <v>13</v>
@@ -4524,10 +4545,10 @@
     </row>
     <row r="129" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
-        <v>45196.970125578708</v>
+        <v>45197.310360416668</v>
       </c>
       <c r="B129" s="3">
-        <v>27538</v>
+        <v>26264</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>14</v>
@@ -4535,28 +4556,28 @@
       <c r="D129" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E129" s="1" t="s">
-        <v>47</v>
+      <c r="E129" s="1">
+        <v>1</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G129" s="1" t="s">
-        <v>140</v>
+        <v>45</v>
+      </c>
+      <c r="G129" s="1">
+        <v>210</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
-        <v>45197.310360416668</v>
+        <v>45197.316604421299</v>
       </c>
       <c r="B130" s="3">
-        <v>26264</v>
+        <v>27995</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>14</v>
@@ -4571,39 +4592,39 @@
         <v>45</v>
       </c>
       <c r="G130" s="1">
-        <v>210</v>
+        <v>3</v>
       </c>
       <c r="H130" s="1" t="s">
-        <v>120</v>
+        <v>54</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
-        <v>45197.316604421299</v>
+        <v>45197.359218229161</v>
       </c>
       <c r="B131" s="3">
-        <v>27995</v>
+        <v>45197</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E131" s="1">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>45</v>
+        <v>110</v>
       </c>
       <c r="G131" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H131" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="I131" s="1" t="s">
         <v>13</v>
@@ -4611,126 +4632,126 @@
     </row>
     <row r="132" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
-        <v>45197.359218229161</v>
+        <v>45197.405554328703</v>
       </c>
       <c r="B132" s="3">
-        <v>45197</v>
+        <v>28735</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="G132" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
-        <v>45197.405554328703</v>
+        <v>45197.472575462962</v>
       </c>
       <c r="B133" s="3">
-        <v>28735</v>
+        <v>23546</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E133" s="1" t="s">
-        <v>47</v>
+        <v>32</v>
+      </c>
+      <c r="E133" s="1">
+        <v>2</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G133" s="1">
         <v>10</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>60</v>
+        <v>143</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
-        <v>45197.472575462962</v>
+        <v>45197.508642314817</v>
       </c>
       <c r="B134" s="3">
-        <v>23546</v>
+        <v>25903</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E134" s="1">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>142</v>
+        <v>51</v>
       </c>
       <c r="G134" s="1">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="H134" s="1" t="s">
-        <v>143</v>
+        <v>92</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
-        <v>45197.508642314817</v>
+        <v>45197.512429571754</v>
       </c>
       <c r="B135" s="3">
-        <v>25903</v>
+        <v>37447</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E135" s="1" t="s">
-        <v>47</v>
+        <v>32</v>
+      </c>
+      <c r="E135" s="1">
+        <v>2</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>51</v>
+        <v>144</v>
       </c>
       <c r="G135" s="1">
-        <v>250</v>
+        <v>420</v>
       </c>
       <c r="H135" s="1" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
-        <v>45197.512429571754</v>
+        <v>45197.553193020838</v>
       </c>
       <c r="B136" s="3">
-        <v>37447</v>
+        <v>29376</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>9</v>
@@ -4738,28 +4759,28 @@
       <c r="D136" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E136" s="1">
-        <v>2</v>
+      <c r="E136" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G136" s="1">
         <v>420</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
-        <v>45197.553193020838</v>
+        <v>45197.594445439812</v>
       </c>
       <c r="B137" s="3">
-        <v>29376</v>
+        <v>29098</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>9</v>
@@ -4771,24 +4792,24 @@
         <v>47</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G137" s="1">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
-        <v>45197.594445439812</v>
+        <v>45197.669844652773</v>
       </c>
       <c r="B138" s="3">
-        <v>29098</v>
+        <v>36785</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>9</v>
@@ -4796,17 +4817,17 @@
       <c r="D138" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E138" s="1" t="s">
-        <v>47</v>
+      <c r="E138" s="1">
+        <v>2</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>146</v>
+        <v>51</v>
       </c>
       <c r="G138" s="1">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="H138" s="1" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="I138" s="1" t="s">
         <v>22</v>
@@ -4814,28 +4835,28 @@
     </row>
     <row r="139" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
-        <v>45197.669844652773</v>
+        <v>45197.673210092587</v>
       </c>
       <c r="B139" s="3">
-        <v>36785</v>
+        <v>37041</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E139" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="G139" s="1">
-        <v>400</v>
+        <v>350</v>
       </c>
       <c r="H139" s="1" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="I139" s="1" t="s">
         <v>22</v>
@@ -4843,68 +4864,68 @@
     </row>
     <row r="140" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
-        <v>45197.673210092587</v>
+        <v>45197.792977777775</v>
       </c>
       <c r="B140" s="3">
-        <v>37041</v>
+        <v>23069</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E140" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="G140" s="1">
-        <v>350</v>
+        <v>10</v>
       </c>
       <c r="H140" s="1" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="141" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
-        <v>45197.792977777775</v>
+        <v>45197.823204803237</v>
       </c>
       <c r="B141" s="3">
-        <v>23069</v>
+        <v>25119</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E141" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G141" s="1">
-        <v>10</v>
+        <v>280</v>
       </c>
       <c r="H141" s="1" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="142" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
-        <v>45197.823204803237</v>
+        <v>45197.887148506939</v>
       </c>
       <c r="B142" s="3">
-        <v>25119</v>
+        <v>26370</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>9</v>
@@ -4913,45 +4934,45 @@
         <v>10</v>
       </c>
       <c r="E142" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>45</v>
+        <v>142</v>
       </c>
       <c r="G142" s="1">
-        <v>280</v>
+        <v>180</v>
       </c>
       <c r="H142" s="1" t="s">
-        <v>120</v>
+        <v>149</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="143" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
-        <v>45197.887148506939</v>
+        <v>45197.900163900464</v>
       </c>
       <c r="B143" s="3">
-        <v>26370</v>
+        <v>34113</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="E143" s="1">
         <v>2</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>142</v>
+        <v>51</v>
       </c>
       <c r="G143" s="1">
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="H143" s="1" t="s">
-        <v>149</v>
+        <v>60</v>
       </c>
       <c r="I143" s="1" t="s">
         <v>13</v>
@@ -4959,28 +4980,28 @@
     </row>
     <row r="144" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
-        <v>45197.900163900464</v>
+        <v>45197.900605694449</v>
       </c>
       <c r="B144" s="3">
-        <v>34113</v>
+        <v>45219</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E144" s="1">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G144" s="1">
-        <v>300</v>
+        <v>45</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="H144" s="1" t="s">
-        <v>60</v>
+        <v>151</v>
       </c>
       <c r="I144" s="1" t="s">
         <v>13</v>
@@ -4988,28 +5009,28 @@
     </row>
     <row r="145" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
-        <v>45197.900605694449</v>
+        <v>45197.902547893522</v>
       </c>
       <c r="B145" s="3">
-        <v>45219</v>
+        <v>33778</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>47</v>
+        <v>32</v>
+      </c>
+      <c r="E145" s="1">
+        <v>2</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G145" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
+      </c>
+      <c r="G145" s="1">
+        <v>450</v>
       </c>
       <c r="H145" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I145" s="1" t="s">
         <v>13</v>
@@ -5017,39 +5038,39 @@
     </row>
     <row r="146" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
-        <v>45197.902547893522</v>
+        <v>45197.903186134259</v>
       </c>
       <c r="B146" s="3">
-        <v>33778</v>
+        <v>32517</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E146" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>152</v>
+        <v>45</v>
       </c>
       <c r="G146" s="1">
-        <v>450</v>
+        <v>265</v>
       </c>
       <c r="H146" s="1" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="147" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
-        <v>45197.903186134259</v>
+        <v>45197.90442126157</v>
       </c>
       <c r="B147" s="3">
-        <v>32517</v>
+        <v>32297</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>9</v>
@@ -5058,27 +5079,27 @@
         <v>32</v>
       </c>
       <c r="E147" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G147" s="1">
-        <v>265</v>
+        <v>51</v>
+      </c>
+      <c r="G147" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="H147" s="1" t="s">
-        <v>112</v>
+        <v>154</v>
       </c>
       <c r="I147" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="148" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
-        <v>45197.90442126157</v>
+        <v>45197.904472997689</v>
       </c>
       <c r="B148" s="3">
-        <v>32297</v>
+        <v>27128</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>9</v>
@@ -5090,53 +5111,53 @@
         <v>2</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H148" s="1" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="I148" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="149" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
-        <v>45197.904472997689</v>
+        <v>45197.906326168981</v>
       </c>
       <c r="B149" s="3">
-        <v>27128</v>
+        <v>33575</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E149" s="1">
         <v>2</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G149" s="1" t="s">
-        <v>155</v>
+        <v>51</v>
+      </c>
+      <c r="G149" s="1">
+        <v>7</v>
       </c>
       <c r="H149" s="1" t="s">
-        <v>138</v>
+        <v>94</v>
       </c>
       <c r="I149" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="150" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
-        <v>45197.906326168981</v>
+        <v>45197.90758298611</v>
       </c>
       <c r="B150" s="3">
-        <v>33575</v>
+        <v>26488</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>9</v>
@@ -5148,13 +5169,13 @@
         <v>2</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G150" s="1">
-        <v>7</v>
+        <v>156</v>
+      </c>
+      <c r="G150" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="H150" s="1" t="s">
-        <v>94</v>
+        <v>158</v>
       </c>
       <c r="I150" s="1" t="s">
         <v>13</v>
@@ -5162,28 +5183,28 @@
     </row>
     <row r="151" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
-        <v>45197.90758298611</v>
+        <v>45197.910743807872</v>
       </c>
       <c r="B151" s="3">
-        <v>26488</v>
+        <v>26849</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E151" s="1">
-        <v>2</v>
+        <v>32</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="G151" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
+      </c>
+      <c r="G151" s="1">
+        <v>8</v>
       </c>
       <c r="H151" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I151" s="1" t="s">
         <v>13</v>
@@ -5191,10 +5212,10 @@
     </row>
     <row r="152" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
-        <v>45197.910743807872</v>
+        <v>45197.91227601852</v>
       </c>
       <c r="B152" s="3">
-        <v>26849</v>
+        <v>35909</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>9</v>
@@ -5202,17 +5223,17 @@
       <c r="D152" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E152" s="1" t="s">
-        <v>47</v>
+      <c r="E152" s="1">
+        <v>1</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G152" s="1">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="G152" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="H152" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I152" s="1" t="s">
         <v>13</v>
@@ -5220,28 +5241,28 @@
     </row>
     <row r="153" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
-        <v>45197.91227601852</v>
+        <v>45197.912979849541</v>
       </c>
       <c r="B153" s="3">
-        <v>35909</v>
+        <v>32416</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E153" s="1">
         <v>1</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G153" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
+      </c>
+      <c r="G153" s="1">
+        <v>120</v>
       </c>
       <c r="H153" s="1" t="s">
-        <v>162</v>
+        <v>80</v>
       </c>
       <c r="I153" s="1" t="s">
         <v>13</v>
@@ -5249,28 +5270,28 @@
     </row>
     <row r="154" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
-        <v>45197.912979849541</v>
+        <v>45197.913158692128</v>
       </c>
       <c r="B154" s="3">
-        <v>32416</v>
+        <v>31026</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E154" s="1">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="G154" s="1">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="H154" s="1" t="s">
-        <v>80</v>
+        <v>21</v>
       </c>
       <c r="I154" s="1" t="s">
         <v>13</v>
@@ -5278,28 +5299,28 @@
     </row>
     <row r="155" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
-        <v>45197.913158692128</v>
+        <v>45197.913990231478</v>
       </c>
       <c r="B155" s="3">
-        <v>31026</v>
+        <v>29939</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>47</v>
+        <v>10</v>
+      </c>
+      <c r="E155" s="1">
+        <v>2</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>142</v>
+        <v>51</v>
       </c>
       <c r="G155" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="H155" s="1" t="s">
-        <v>21</v>
+        <v>164</v>
       </c>
       <c r="I155" s="1" t="s">
         <v>13</v>
@@ -5307,39 +5328,39 @@
     </row>
     <row r="156" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
-        <v>45197.913990231478</v>
+        <v>45197.917245810182</v>
       </c>
       <c r="B156" s="3">
-        <v>29939</v>
+        <v>29830</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="E156" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G156" s="1">
-        <v>180</v>
+        <v>330</v>
       </c>
       <c r="H156" s="1" t="s">
-        <v>164</v>
+        <v>58</v>
       </c>
       <c r="I156" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="157" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
-        <v>45197.917245810182</v>
+        <v>45197.922624687504</v>
       </c>
       <c r="B157" s="3">
-        <v>29830</v>
+        <v>30568</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>14</v>
@@ -5348,85 +5369,85 @@
         <v>32</v>
       </c>
       <c r="E157" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G157" s="1">
-        <v>330</v>
+        <v>400</v>
       </c>
       <c r="H157" s="1" t="s">
-        <v>58</v>
+        <v>162</v>
       </c>
       <c r="I157" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="158" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
-        <v>45197.922624687504</v>
+        <v>45197.923034606487</v>
       </c>
       <c r="B158" s="3">
-        <v>30568</v>
+        <v>32735</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E158" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="G158" s="1">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="H158" s="1" t="s">
-        <v>162</v>
+        <v>21</v>
       </c>
       <c r="I158" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="159" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
-        <v>45197.923034606487</v>
+        <v>45197.926504618052</v>
       </c>
       <c r="B159" s="3">
-        <v>32735</v>
+        <v>32458</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E159" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>21</v>
+        <v>142</v>
       </c>
       <c r="G159" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="H159" s="1" t="s">
-        <v>21</v>
+        <v>165</v>
       </c>
       <c r="I159" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
-        <v>45197.926504618052</v>
+        <v>45197.928490081016</v>
       </c>
       <c r="B160" s="3">
-        <v>32458</v>
+        <v>28529</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>9</v>
@@ -5438,13 +5459,13 @@
         <v>2</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>142</v>
+        <v>51</v>
       </c>
       <c r="G160" s="1">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="H160" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I160" s="1" t="s">
         <v>13</v>
@@ -5452,74 +5473,74 @@
     </row>
     <row r="161" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
-        <v>45197.928490081016</v>
+        <v>45197.936815416666</v>
       </c>
       <c r="B161" s="3">
-        <v>28529</v>
+        <v>34228</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E161" s="1">
-        <v>2</v>
+        <v>32</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="G161" s="1">
-        <v>160</v>
+        <v>360</v>
       </c>
       <c r="H161" s="1" t="s">
-        <v>166</v>
+        <v>25</v>
       </c>
       <c r="I161" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="162" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
-        <v>45197.936815416666</v>
+        <v>45197.946119583328</v>
       </c>
       <c r="B162" s="3">
-        <v>34228</v>
+        <v>33586</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D162" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E162" s="1" t="s">
-        <v>47</v>
+      <c r="E162" s="1">
+        <v>1</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>146</v>
+        <v>45</v>
       </c>
       <c r="G162" s="1">
-        <v>360</v>
+        <v>240</v>
       </c>
       <c r="H162" s="1" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="I162" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
-        <v>45197.946119583328</v>
+        <v>45197.946977071755</v>
       </c>
       <c r="B163" s="3">
-        <v>33586</v>
+        <v>27814</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E163" s="1">
         <v>1</v>
@@ -5528,10 +5549,10 @@
         <v>45</v>
       </c>
       <c r="G163" s="1">
-        <v>240</v>
+        <v>60</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>92</v>
+        <v>167</v>
       </c>
       <c r="I163" s="1" t="s">
         <v>13</v>
@@ -5539,39 +5560,39 @@
     </row>
     <row r="164" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
-        <v>45197.946977071755</v>
+        <v>45197.94721672454</v>
       </c>
       <c r="B164" s="3">
-        <v>27814</v>
+        <v>30213</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E164" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>45</v>
+        <v>142</v>
       </c>
       <c r="G164" s="1">
-        <v>60</v>
+        <v>210</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>167</v>
+        <v>120</v>
       </c>
       <c r="I164" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="165" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
-        <v>45197.94721672454</v>
+        <v>45197.960053530092</v>
       </c>
       <c r="B165" s="3">
-        <v>30213</v>
+        <v>27537</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>9</v>
@@ -5579,46 +5600,46 @@
       <c r="D165" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E165" s="1">
-        <v>2</v>
+      <c r="E165" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="G165" s="1">
-        <v>210</v>
+        <v>18</v>
+      </c>
+      <c r="G165" s="1" t="s">
+        <v>168</v>
       </c>
       <c r="H165" s="1" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="I165" s="1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="166" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
-        <v>45197.960053530092</v>
+        <v>45197.961574224537</v>
       </c>
       <c r="B166" s="3">
-        <v>27537</v>
+        <v>23680</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>47</v>
+        <v>32</v>
+      </c>
+      <c r="E166" s="1">
+        <v>2</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G166" s="1" t="s">
-        <v>168</v>
+        <v>111</v>
+      </c>
+      <c r="G166" s="1">
+        <v>8</v>
       </c>
       <c r="H166" s="1" t="s">
-        <v>88</v>
+        <v>169</v>
       </c>
       <c r="I166" s="1" t="s">
         <v>13</v>
@@ -5626,45 +5647,45 @@
     </row>
     <row r="167" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
-        <v>45197.961574224537</v>
+        <v>45197.962478773145</v>
       </c>
       <c r="B167" s="3">
-        <v>23680</v>
+        <v>25346</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E167" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>111</v>
+        <v>45</v>
       </c>
       <c r="G167" s="1">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="H167" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I167" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="168" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
-        <v>45197.962478773145</v>
+        <v>45197.976489583336</v>
       </c>
       <c r="B168" s="3">
-        <v>25346</v>
+        <v>45200</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="E168" s="1">
         <v>1</v>
@@ -5673,108 +5694,108 @@
         <v>45</v>
       </c>
       <c r="G168" s="1">
-        <v>120</v>
+        <v>480</v>
       </c>
       <c r="H168" s="1" t="s">
-        <v>170</v>
+        <v>112</v>
       </c>
       <c r="I168" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="169" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
-        <v>45197.976489583336</v>
+        <v>45198.034582048611</v>
       </c>
       <c r="B169" s="3">
-        <v>45200</v>
+        <v>44948</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D169" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E169" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G169" s="1">
-        <v>480</v>
+        <v>111</v>
+      </c>
+      <c r="G169" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="H169" s="1" t="s">
-        <v>112</v>
+        <v>162</v>
       </c>
       <c r="I169" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="170" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
-        <v>45198.034582048611</v>
+        <v>45198.044565358796</v>
       </c>
       <c r="B170" s="3">
-        <v>44948</v>
+        <v>26598</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E170" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G170" s="1" t="s">
-        <v>171</v>
+        <v>45</v>
+      </c>
+      <c r="G170" s="1">
+        <v>3</v>
       </c>
       <c r="H170" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="I170" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
-        <v>45198.044565358796</v>
+        <v>45198.304530601847</v>
       </c>
       <c r="B171" s="3">
-        <v>26598</v>
+        <v>21813</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E171" s="1">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G171" s="1">
-        <v>3</v>
+        <v>146</v>
+      </c>
+      <c r="G171" s="1" t="s">
+        <v>172</v>
       </c>
       <c r="H171" s="1" t="s">
-        <v>158</v>
+        <v>40</v>
       </c>
       <c r="I171" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="172" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
-        <v>45198.304530601847</v>
+        <v>45198.308512291667</v>
       </c>
       <c r="B172" s="3">
-        <v>21813</v>
+        <v>33636</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>9</v>
@@ -5786,76 +5807,48 @@
         <v>47</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G172" s="1" t="s">
-        <v>172</v>
+        <v>142</v>
+      </c>
+      <c r="G172" s="1">
+        <v>300</v>
       </c>
       <c r="H172" s="1" t="s">
-        <v>40</v>
+        <v>138</v>
       </c>
       <c r="I172" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
-        <v>45198.308512291667</v>
+        <v>45198.898450081018</v>
       </c>
       <c r="B173" s="3">
-        <v>33636</v>
+        <v>23124</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D173" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E173" s="1" t="s">
-        <v>47</v>
+      <c r="E173" s="1">
+        <v>2</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="G173" s="1">
-        <v>300</v>
+        <v>111</v>
+      </c>
+      <c r="G173" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="H173" s="1" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
       <c r="I173" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="174" spans="1:9" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A174" s="2">
-        <v>45198.898450081018</v>
-      </c>
-      <c r="B174" s="3">
-        <v>23124</v>
-      </c>
-      <c r="C174" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D174" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E174" s="1">
-        <v>2</v>
-      </c>
-      <c r="F174" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G174" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="H174" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I174" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
+    <row r="174" spans="1:9" ht="12.5" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>